<commit_message>
Apresentacao Casos Práticos adicionados
</commit_message>
<xml_diff>
--- a/Documents/simulacaodoentes.xlsx
+++ b/Documents/simulacaodoentes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaob\OneDrive\Ambiente de Trabalho\UBI\3 2S\COPDMobileApp-UBI\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037F4019-4F41-4676-814D-357FEA1E4C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB98FF8B-AC71-4838-A544-F6A0C78F9304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E78E22FD-07D3-4E4D-B139-0900B51A46B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{E78E22FD-07D3-4E4D-B139-0900B51A46B9}"/>
   </bookViews>
   <sheets>
     <sheet name="parâmetros" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
   <si>
     <t>pO2</t>
   </si>
@@ -213,6 +213,30 @@
   </si>
   <si>
     <t xml:space="preserve">     VARIABLES:0.0</t>
+  </si>
+  <si>
+    <t>Ultimas 19</t>
+  </si>
+  <si>
+    <t>Ultimas 07</t>
+  </si>
+  <si>
+    <t>Ultimas 5:15</t>
+  </si>
+  <si>
+    <t>Ultimas 5:30</t>
+  </si>
+  <si>
+    <t>Ultimas 5:45</t>
+  </si>
+  <si>
+    <t>Imaginemos que está às 23:08</t>
+  </si>
+  <si>
+    <t>:30</t>
+  </si>
+  <si>
+    <t>Ultimas 14</t>
   </si>
 </sst>
 </file>
@@ -794,10 +818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD57B25B-20E9-4C32-8EAF-71987A85E754}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1272,6 +1296,44 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
     </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1282,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3E3826-57EF-4325-8BC1-59CC34AE98EA}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H32" activeCellId="1" sqref="K35 H32:L35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Preparacao apresentacao afinar dados paciente
</commit_message>
<xml_diff>
--- a/Documents/simulacaodoentes.xlsx
+++ b/Documents/simulacaodoentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaob\OneDrive\Ambiente de Trabalho\UBI\3 2S\COPDMobileApp-UBI\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB98FF8B-AC71-4838-A544-F6A0C78F9304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D79205-E43F-494E-9878-BC0D36DB2561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{E78E22FD-07D3-4E4D-B139-0900B51A46B9}"/>
   </bookViews>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD57B25B-20E9-4C32-8EAF-71987A85E754}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -890,10 +890,7 @@
         <v>38</v>
       </c>
       <c r="I4">
-        <v>7</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1344,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3E3826-57EF-4325-8BC1-59CC34AE98EA}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,10 +1411,7 @@
         <v>38</v>
       </c>
       <c r="I4">
-        <v>33</v>
-      </c>
-      <c r="J4">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>